<commit_message>
Final records individual added
</commit_message>
<xml_diff>
--- a/data/MF201601_Final.xlsx
+++ b/data/MF201601_Final.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Park Min Suk\Desktop\수업자료\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coop2711/Google 드라이브/Works/Class/Math_Foundations/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7710"/>
+    <workbookView xWindow="31060" yWindow="1460" windowWidth="20500" windowHeight="14780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -310,55 +316,55 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -366,10 +372,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -433,7 +439,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="기본" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -494,9 +500,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -529,9 +535,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -713,13 +719,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>51</v>
       </c>
@@ -727,7 +733,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>48</v>
       </c>
@@ -745,15 +751,15 @@
       </c>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C4" s="8">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E4" s="10">
         <v>90</v>
@@ -766,18 +772,18 @@
         <v>60.11904761904762</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C5" s="8">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E5" s="10">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>43</v>
@@ -787,18 +793,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="C6" s="8">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="E6" s="10">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>44</v>
@@ -808,18 +814,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7" s="8">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7" s="10">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>50</v>
@@ -829,529 +835,529 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="8">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" s="10">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2013</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="E9" s="10">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C10" s="8">
         <v>2013</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E10" s="10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C11" s="8">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E11" s="10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C12" s="8">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C13" s="8">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="10">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C14" s="8">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E14" s="10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C15" s="8">
         <v>2013</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
+        <v>36</v>
+      </c>
+      <c r="C16" s="8">
+        <v>2013</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
+        <v>37</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2014</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
+        <v>38</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2014</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B19" s="7">
+        <v>2</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B21" s="7">
+        <v>4</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B22" s="7">
+        <v>5</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B23" s="7">
         <v>6</v>
       </c>
-      <c r="E15" s="10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B16" s="7">
+      <c r="C23" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B24" s="7">
+        <v>8</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
+        <v>9</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
+        <v>10</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
+        <v>11</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
         <v>13</v>
       </c>
-      <c r="C16" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C28" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E28" s="10">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B17" s="7">
+    <row r="29" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B29" s="7">
         <v>14</v>
       </c>
-      <c r="C17" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D17" s="9" t="s">
+      <c r="C29" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E29" s="10">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B18" s="7">
+    <row r="30" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
         <v>15</v>
       </c>
-      <c r="C18" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="C30" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E30" s="10">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B19" s="7">
+    <row r="31" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B31" s="7">
         <v>16</v>
       </c>
-      <c r="C19" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="C31" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E31" s="10">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B20" s="7">
+    <row r="32" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B32" s="7">
         <v>17</v>
       </c>
-      <c r="C20" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="C32" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E32" s="10">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B21" s="7">
-        <v>18</v>
-      </c>
-      <c r="C21" s="8">
-        <v>2013</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="10">
+    <row r="33" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B33" s="7">
+        <v>19</v>
+      </c>
+      <c r="C33" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B34" s="7">
+        <v>21</v>
+      </c>
+      <c r="C34" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B35" s="7">
+        <v>22</v>
+      </c>
+      <c r="C35" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B36" s="7">
+        <v>24</v>
+      </c>
+      <c r="C36" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B37" s="7">
+        <v>25</v>
+      </c>
+      <c r="C37" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B38" s="7">
+        <v>26</v>
+      </c>
+      <c r="C38" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B39" s="7">
+        <v>28</v>
+      </c>
+      <c r="C39" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B40" s="7">
+        <v>29</v>
+      </c>
+      <c r="C40" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="10">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B22" s="7">
-        <v>19</v>
-      </c>
-      <c r="C22" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D22" s="9" t="s">
+    <row r="41" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B41" s="7">
+        <v>30</v>
+      </c>
+      <c r="C41" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B42" s="7">
+        <v>32</v>
+      </c>
+      <c r="C42" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B43" s="7">
+        <v>34</v>
+      </c>
+      <c r="C43" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B44" s="7">
         <v>35</v>
       </c>
-      <c r="E22" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B23" s="7">
-        <v>20</v>
-      </c>
-      <c r="C23" s="8">
-        <v>2013</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="10">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B24" s="7">
-        <v>21</v>
-      </c>
-      <c r="C24" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="10">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B25" s="7">
-        <v>22</v>
-      </c>
-      <c r="C25" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="10">
+      <c r="C44" s="8">
+        <v>2015</v>
+      </c>
+      <c r="D44" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B26" s="7">
-        <v>23</v>
-      </c>
-      <c r="C26" s="8">
-        <v>2013</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B27" s="7">
-        <v>24</v>
-      </c>
-      <c r="C27" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B28" s="7">
-        <v>25</v>
-      </c>
-      <c r="C28" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B29" s="7">
-        <v>26</v>
-      </c>
-      <c r="C29" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="10">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B30" s="7">
-        <v>27</v>
-      </c>
-      <c r="C30" s="8">
-        <v>2013</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B31" s="7">
-        <v>28</v>
-      </c>
-      <c r="C31" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B32" s="7">
-        <v>29</v>
-      </c>
-      <c r="C32" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="10">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B33" s="7">
-        <v>30</v>
-      </c>
-      <c r="C33" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="10">
+      <c r="E44" s="10">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B34" s="7">
-        <v>31</v>
-      </c>
-      <c r="C34" s="8">
-        <v>2013</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B35" s="7">
-        <v>32</v>
-      </c>
-      <c r="C35" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B36" s="7">
-        <v>33</v>
-      </c>
-      <c r="C36" s="8">
-        <v>2013</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="10">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B37" s="7">
-        <v>34</v>
-      </c>
-      <c r="C37" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="10">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B38" s="7">
-        <v>35</v>
-      </c>
-      <c r="C38" s="8">
-        <v>2015</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" s="10">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B39" s="7">
-        <v>36</v>
-      </c>
-      <c r="C39" s="8">
-        <v>2013</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B40" s="7">
-        <v>37</v>
-      </c>
-      <c r="C40" s="8">
-        <v>2014</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B41" s="7">
-        <v>38</v>
-      </c>
-      <c r="C41" s="8">
-        <v>2014</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B42" s="7">
-        <v>39</v>
-      </c>
-      <c r="C42" s="8">
-        <v>2009</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B43" s="7">
-        <v>40</v>
-      </c>
-      <c r="C43" s="8">
-        <v>2011</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E43" s="10">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B44" s="7">
-        <v>41</v>
-      </c>
-      <c r="C44" s="8">
-        <v>2011</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E44" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" ht="18" x14ac:dyDescent="0.25">
       <c r="B45" s="7">
         <v>42</v>
       </c>
@@ -1368,7 +1374,7 @@
   </sheetData>
   <autoFilter ref="B3:E3">
     <sortState ref="B4:E45">
-      <sortCondition ref="B3"/>
+      <sortCondition ref="C3:C45"/>
     </sortState>
   </autoFilter>
   <mergeCells count="2">

</xml_diff>